<commit_message>
LAB 03-03 to LAB 03-04 UPDATE
</commit_message>
<xml_diff>
--- a/Lab 03/diglab_03_04/diglab_03_04_pics/diglab_03_04_table.xlsx
+++ b/Lab 03/diglab_03_04/diglab_03_04_pics/diglab_03_04_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\College Year 2\2110263 DIG LOGIC LAB I\2110263-DIG-LOGIC-LAB-I\Lab 03\diglab_03_04\diglab_03_04_pics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868F784F-A355-4DE4-9ADA-367014B1C9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E446488-1FFC-4B51-A880-C34029AD45F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2F5C648-1E30-482C-A813-F5047B4D4EC4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E2F5C648-1E30-482C-A813-F5047B4D4EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Circuit A" sheetId="7" r:id="rId1"/>
@@ -582,6 +582,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,61 +627,34 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86236B5-ED94-4827-B61A-9172EEC20567}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -985,10 +985,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
@@ -1002,7 +1002,7 @@
       <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="34" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="35" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1018,7 +1018,7 @@
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="35" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1046,36 +1046,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="44"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
+      <c r="A2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="43"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCAF7C92-3A04-4E34-9DD3-DA209B62F3C4}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1424,91 +1424,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="44"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="30"/>
+      <c r="A2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39"/>
       <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="30"/>
+      <c r="D2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="39"/>
       <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="30"/>
+      <c r="G2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="39"/>
       <c r="I2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="30"/>
+      <c r="J2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="39"/>
       <c r="L2" s="27" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="41" t="s">
+      <c r="L3" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42">
+      <c r="A4" s="32">
         <v>0</v>
       </c>
       <c r="B4" s="2">
@@ -1517,7 +1517,7 @@
       <c r="C4" s="22">
         <v>0</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="32">
         <v>0</v>
       </c>
       <c r="E4" s="2">
@@ -1526,7 +1526,7 @@
       <c r="F4" s="22">
         <v>0</v>
       </c>
-      <c r="G4" s="42">
+      <c r="G4" s="32">
         <v>0</v>
       </c>
       <c r="H4" s="2">
@@ -1535,7 +1535,7 @@
       <c r="I4" s="22">
         <v>0</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="32">
         <v>0</v>
       </c>
       <c r="K4" s="2">
@@ -1546,7 +1546,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42">
+      <c r="A5" s="32">
         <v>0</v>
       </c>
       <c r="B5" s="2">
@@ -1555,7 +1555,7 @@
       <c r="C5" s="22">
         <v>1</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="32">
         <v>0</v>
       </c>
       <c r="E5" s="2">
@@ -1564,7 +1564,7 @@
       <c r="F5" s="22">
         <v>1</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="32">
         <v>0</v>
       </c>
       <c r="H5" s="2">
@@ -1573,7 +1573,7 @@
       <c r="I5" s="22">
         <v>1</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="32">
         <v>0</v>
       </c>
       <c r="K5" s="2">
@@ -1584,7 +1584,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42">
+      <c r="A6" s="32">
         <v>1</v>
       </c>
       <c r="B6" s="2">
@@ -1593,7 +1593,7 @@
       <c r="C6" s="22">
         <v>1</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="32">
         <v>1</v>
       </c>
       <c r="E6" s="2">
@@ -1602,7 +1602,7 @@
       <c r="F6" s="22">
         <v>1</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="32">
         <v>1</v>
       </c>
       <c r="H6" s="2">
@@ -1611,7 +1611,7 @@
       <c r="I6" s="22">
         <v>1</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="32">
         <v>1</v>
       </c>
       <c r="K6" s="2">
@@ -1622,7 +1622,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="44">
+      <c r="A7" s="33">
         <v>1</v>
       </c>
       <c r="B7" s="6">
@@ -1631,7 +1631,7 @@
       <c r="C7" s="24">
         <v>0</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="33">
         <v>1</v>
       </c>
       <c r="E7" s="6">
@@ -1640,7 +1640,7 @@
       <c r="F7" s="24">
         <v>0</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="33">
         <v>1</v>
       </c>
       <c r="H7" s="6">
@@ -1649,7 +1649,7 @@
       <c r="I7" s="24">
         <v>0</v>
       </c>
-      <c r="J7" s="44">
+      <c r="J7" s="33">
         <v>1</v>
       </c>
       <c r="K7" s="6">
@@ -1660,65 +1660,65 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="30"/>
+      <c r="A8" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="39"/>
       <c r="C8" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="30"/>
+      <c r="D8" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="39"/>
       <c r="F8" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="30"/>
+      <c r="G8" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="39"/>
       <c r="I8" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="48"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="47"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="50"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="43"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="50"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42">
+      <c r="A10" s="32">
         <v>0</v>
       </c>
       <c r="B10" s="2">
@@ -1727,7 +1727,7 @@
       <c r="C10" s="22">
         <v>0</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="32">
         <v>0</v>
       </c>
       <c r="E10" s="2">
@@ -1736,7 +1736,7 @@
       <c r="F10" s="22">
         <v>0</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="32">
         <v>0</v>
       </c>
       <c r="H10" s="2">
@@ -1745,12 +1745,12 @@
       <c r="I10" s="22">
         <v>0</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="43"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="50"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42">
+      <c r="A11" s="32">
         <v>0</v>
       </c>
       <c r="B11" s="2">
@@ -1759,7 +1759,7 @@
       <c r="C11" s="22">
         <v>1</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="32">
         <v>0</v>
       </c>
       <c r="E11" s="2">
@@ -1768,7 +1768,7 @@
       <c r="F11" s="22">
         <v>1</v>
       </c>
-      <c r="G11" s="42">
+      <c r="G11" s="32">
         <v>0</v>
       </c>
       <c r="H11" s="2">
@@ -1777,12 +1777,12 @@
       <c r="I11" s="22">
         <v>1</v>
       </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="43"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="50"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42">
+      <c r="A12" s="32">
         <v>1</v>
       </c>
       <c r="B12" s="2">
@@ -1791,7 +1791,7 @@
       <c r="C12" s="22">
         <v>1</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="32">
         <v>1</v>
       </c>
       <c r="E12" s="2">
@@ -1800,7 +1800,7 @@
       <c r="F12" s="22">
         <v>1</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="32">
         <v>1</v>
       </c>
       <c r="H12" s="2">
@@ -1809,12 +1809,12 @@
       <c r="I12" s="22">
         <v>1</v>
       </c>
-      <c r="J12" s="50"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="43"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="50"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="44">
+      <c r="A13" s="33">
         <v>1</v>
       </c>
       <c r="B13" s="6">
@@ -1823,7 +1823,7 @@
       <c r="C13" s="24">
         <v>0</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="33">
         <v>1</v>
       </c>
       <c r="E13" s="6">
@@ -1832,7 +1832,7 @@
       <c r="F13" s="24">
         <v>0</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="33">
         <v>1</v>
       </c>
       <c r="H13" s="6">
@@ -1842,8 +1842,8 @@
         <v>0</v>
       </c>
       <c r="J13" s="51"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="46"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>